<commit_message>
Add custom formatter for tests: CustomBooleanFormatter
</commit_message>
<xml_diff>
--- a/src/test/resources/sample/sample.xlsx
+++ b/src/test/resources/sample/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>b</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>г</t>
+  </si>
+  <si>
+    <t>Custom boolean</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Нет</t>
   </si>
 </sst>
 </file>
@@ -394,10 +403,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:I1000"/>
+  <dimension ref="A2:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -409,7 +418,7 @@
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -434,8 +443,11 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -463,8 +475,11 @@
       <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -488,8 +503,11 @@
       <c r="I4" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -514,8 +532,11 @@
       <c r="I5" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>40</v>
@@ -538,8 +559,11 @@
       <c r="I6" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H7" t="s">
         <v>11</v>
       </c>
@@ -547,7 +571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="5">
         <v>45209</v>
       </c>
@@ -555,7 +579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -584,7 +608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>602436346346.33496</v>
       </c>
@@ -602,7 +626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C11">
         <f>IF(100 &gt;C5,5,6)</f>
         <v>6</v>
@@ -615,28 +639,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E12" s="4"/>
       <c r="H12" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E13" s="4"/>
       <c r="H13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E14" s="4"/>
       <c r="H14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E16" s="4"/>
       <c r="H16" s="6" t="s">
         <v>21</v>

</xml_diff>